<commit_message>
lodgepole forest graphs and some adjustment on burnt chopped wood
</commit_message>
<xml_diff>
--- a/data/clean/lodgepole_forest.xlsx
+++ b/data/clean/lodgepole_forest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Katie Frazer\Documents\ESS500_ForestCarbon\data\clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C7062C-A856-445F-8455-FB1636A0DE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CED2553-358A-4E9D-AE8C-79799B8DF91D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="17472" windowHeight="10992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="17472" windowHeight="10992" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="F24 % Cover" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="52">
   <si>
     <t>Grass</t>
   </si>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t># of event occurred / # of events it could occur</t>
+  </si>
+  <si>
+    <t>GroundCover</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -520,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1409,7 +1415,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1420,6 +1426,9 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
       <c r="B2">
         <v>1996</v>
       </c>
@@ -1650,8 +1659,8 @@
       <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="s">
-        <v>20</v>
+      <c r="C9">
+        <v>0</v>
       </c>
       <c r="D9">
         <v>25</v>
@@ -1702,7 +1711,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1713,6 +1722,9 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
       <c r="B2">
         <v>1996</v>
       </c>
@@ -1773,8 +1785,7 @@
         <v>3.6</v>
       </c>
       <c r="K3" s="2">
-        <f>(3/29)*100</f>
-        <v>10.344827586206897</v>
+        <v>10.3</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1806,8 +1817,7 @@
         <v>17.899999999999999</v>
       </c>
       <c r="K4" s="2">
-        <f>(4/29)*100</f>
-        <v>13.793103448275861</v>
+        <v>13.8</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1839,8 +1849,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="2">
-        <f>(5/29)*100</f>
-        <v>17.241379310344829</v>
+        <v>17.2</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1872,8 +1881,7 @@
         <v>3.6</v>
       </c>
       <c r="K6" s="2">
-        <f>(1/29)*100</f>
-        <v>3.4482758620689653</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1905,8 +1913,7 @@
         <v>17.600000000000001</v>
       </c>
       <c r="K7" s="2">
-        <f>(6/29)*100</f>
-        <v>20.689655172413794</v>
+        <v>20.7</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1938,8 +1945,7 @@
         <v>17.600000000000001</v>
       </c>
       <c r="K8" s="2">
-        <f>(8/29)*100</f>
-        <v>27.586206896551722</v>
+        <v>27.6</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1949,8 +1955,8 @@
       <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="s">
-        <v>20</v>
+      <c r="C9">
+        <v>0</v>
       </c>
       <c r="D9">
         <v>8</v>
@@ -1958,6 +1964,9 @@
       <c r="E9">
         <v>20</v>
       </c>
+      <c r="F9" t="s">
+        <v>51</v>
+      </c>
       <c r="G9">
         <v>16.7</v>
       </c>
@@ -1971,8 +1980,7 @@
         <v>25</v>
       </c>
       <c r="K9" s="2">
-        <f>(2/29)*100</f>
-        <v>6.8965517241379306</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2006,8 +2014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E67D1C-38E2-44AC-A628-4FD21994B438}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2018,6 +2026,9 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
       <c r="B2">
         <v>1996</v>
       </c>
@@ -2078,7 +2089,7 @@
         <v>5</v>
       </c>
       <c r="K3" s="2">
-        <v>5.025125628140704</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2110,7 +2121,7 @@
         <v>7.5</v>
       </c>
       <c r="K4" s="2">
-        <v>4.1206030150753765</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2142,7 +2153,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="2">
-        <v>20.603015075376884</v>
+        <v>20.6</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2174,7 +2185,7 @@
         <v>4</v>
       </c>
       <c r="K6" s="2">
-        <v>3.0150753768844218</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2206,7 +2217,7 @@
         <v>29</v>
       </c>
       <c r="K7" s="2">
-        <v>19.698492462311556</v>
+        <v>19.7</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2270,7 +2281,7 @@
         <v>23.5</v>
       </c>
       <c r="K9" s="2">
-        <v>7.5376884422110546</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">

</xml_diff>